<commit_message>
shivanisantoshwar: hlookup and documentadd for v and h lookup
</commit_message>
<xml_diff>
--- a/day11.xlsx
+++ b/day11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462E1E3F-DB5D-4263-A4EF-2D71EAABBC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A672CB-185B-4DAB-B5D4-36C08E38E70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1729F0FB-929A-46E2-8634-558E4EC6404C}"/>
   </bookViews>
@@ -778,7 +778,7 @@
   <dimension ref="D10:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:J14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,12 +819,30 @@
       <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="E11" s="3" t="str">
+        <f>HLOOKUP(E10,$D$20:$J$22,2,)</f>
+        <v>automotive sq near tp road, 400001</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f t="shared" ref="F11:J11" si="0">HLOOKUP(F10,$D$20:$J$22,2,)</f>
+        <v>offline</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
@@ -876,12 +894,30 @@
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="E14" s="3" t="str">
+        <f>HLOOKUP(E10,$D$20:$J$22,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f>HLOOKUP(F10,$D$20:$J$22,3,FALSE)</f>
+        <v>online</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" ref="G14:J14" si="1">HLOOKUP(G10,$D$20:$J$22,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">

</xml_diff>